<commit_message>
minor change, pulled from dev to deploy latest changes aswell
</commit_message>
<xml_diff>
--- a/Web/db_data/testarticles.xlsx
+++ b/Web/db_data/testarticles.xlsx
@@ -27,7 +27,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>supplier</t>
+    <t>supplier_id</t>
   </si>
   <si>
     <t>supplier_article_nr</t>
@@ -390,7 +390,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">

</xml_diff>

<commit_message>
issues, Ive got isses
</commit_message>
<xml_diff>
--- a/Web/db_data/testarticles.xlsx
+++ b/Web/db_data/testarticles.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miS6lotPXKaktnpKtMkmSKVupqL7Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miUu12gx9a5lNIYm3z3FkbCpeQP0A=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>lio_id</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>Min. ord.kvant.</t>
   </si>
   <si>
     <t>article_group</t>
@@ -372,12 +369,11 @@
     <col customWidth="1" min="5" max="5" width="17.57"/>
     <col customWidth="1" min="6" max="6" width="6.43"/>
     <col customWidth="1" min="7" max="7" width="10.43"/>
-    <col customWidth="1" min="8" max="8" width="17.0"/>
-    <col customWidth="1" min="9" max="9" width="13.14"/>
-    <col customWidth="1" min="10" max="10" width="13.71"/>
-    <col customWidth="1" min="11" max="11" width="15.71"/>
-    <col customWidth="1" min="12" max="12" width="12.86"/>
-    <col customWidth="1" min="13" max="24" width="45.14"/>
+    <col customWidth="1" min="8" max="8" width="13.14"/>
+    <col customWidth="1" min="9" max="9" width="13.71"/>
+    <col customWidth="1" min="10" max="10" width="15.71"/>
+    <col customWidth="1" min="11" max="11" width="12.86"/>
+    <col customWidth="1" min="12" max="23" width="45.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -402,10 +398,10 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -413,9 +409,6 @@
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -423,7 +416,7 @@
         <v>778801.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="str">
         <f t="shared" ref="C2:C14" si="1">B2</f>
@@ -439,17 +432,14 @@
       <c r="G2" s="5">
         <v>29.0</v>
       </c>
-      <c r="H2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I2" s="5">
+      <c r="H2" s="5">
         <v>101.0</v>
       </c>
-      <c r="K2" s="3">
+      <c r="J2" s="3">
         <v>10.0</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>13</v>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +447,7 @@
         <v>778802.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" si="1"/>
@@ -473,20 +463,17 @@
       <c r="G3" s="5">
         <v>39.0</v>
       </c>
-      <c r="H3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="H3" s="5">
         <v>101.0</v>
       </c>
-      <c r="J3" s="3" t="b">
+      <c r="I3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K3" s="3">
+      <c r="J3" s="3">
         <v>10.0</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>13</v>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +481,7 @@
         <v>778803.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="1"/>
@@ -510,17 +497,14 @@
       <c r="G4" s="5">
         <v>19.0</v>
       </c>
-      <c r="H4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="H4" s="5">
         <v>101.0</v>
       </c>
-      <c r="K4" s="3">
+      <c r="J4" s="3">
         <v>100.0</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>13</v>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -528,7 +512,7 @@
         <v>778804.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="1"/>
@@ -544,17 +528,14 @@
       <c r="G5" s="5">
         <v>19.0</v>
       </c>
-      <c r="H5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="H5" s="5">
         <v>101.0</v>
       </c>
-      <c r="K5" s="3">
+      <c r="J5" s="3">
         <v>100.0</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>13</v>
+      <c r="K5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -562,7 +543,7 @@
         <v>778805.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="1"/>
@@ -576,17 +557,14 @@
       <c r="G6" s="5">
         <v>19.0</v>
       </c>
-      <c r="H6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="5">
         <v>101.0</v>
       </c>
-      <c r="K6" s="3">
+      <c r="J6" s="3">
         <v>25.0</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>13</v>
+      <c r="K6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -594,7 +572,7 @@
         <v>778806.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="1"/>
@@ -610,17 +588,14 @@
       <c r="G7" s="5">
         <v>29.0</v>
       </c>
-      <c r="H7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="H7" s="5">
         <v>101.0</v>
       </c>
-      <c r="K7" s="3">
+      <c r="J7" s="3">
         <v>10.0</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>13</v>
+      <c r="K7" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -628,7 +603,7 @@
         <v>778807.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="1"/>
@@ -644,20 +619,17 @@
       <c r="G8" s="5">
         <v>19.0</v>
       </c>
-      <c r="H8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="H8" s="5">
         <v>101.0</v>
       </c>
-      <c r="J8" s="3" t="b">
+      <c r="I8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="3">
+      <c r="J8" s="3">
         <v>10.0</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>13</v>
+      <c r="K8" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -665,7 +637,7 @@
         <v>778808.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="1"/>
@@ -681,20 +653,17 @@
       <c r="G9" s="5">
         <v>39.0</v>
       </c>
-      <c r="H9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="H9" s="5">
         <v>101.0</v>
       </c>
-      <c r="J9" s="3" t="b">
+      <c r="I9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K9" s="3">
+      <c r="J9" s="3">
         <v>20.0</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>13</v>
+      <c r="K9" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -702,7 +671,7 @@
         <v>778809.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="1"/>
@@ -718,20 +687,17 @@
       <c r="G10" s="3">
         <v>29.0</v>
       </c>
-      <c r="H10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="H10" s="5">
         <v>101.0</v>
       </c>
-      <c r="J10" s="3" t="b">
+      <c r="I10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K10" s="3">
+      <c r="J10" s="3">
         <v>20.0</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>13</v>
+      <c r="K10" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -739,7 +705,7 @@
         <v>778810.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="1"/>
@@ -755,17 +721,14 @@
       <c r="G11" s="5">
         <v>39.0</v>
       </c>
-      <c r="H11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="H11" s="5">
         <v>101.0</v>
       </c>
-      <c r="K11" s="3">
+      <c r="J11" s="3">
         <v>20.0</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>13</v>
+      <c r="K11" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -773,7 +736,7 @@
         <v>778811.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" si="1"/>
@@ -789,17 +752,14 @@
       <c r="G12" s="5">
         <v>39.0</v>
       </c>
-      <c r="H12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="H12" s="5">
         <v>101.0</v>
       </c>
-      <c r="K12" s="3">
+      <c r="J12" s="3">
         <v>250.0</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>13</v>
+      <c r="K12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -807,7 +767,7 @@
         <v>778812.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="1"/>
@@ -823,20 +783,17 @@
       <c r="G13" s="5">
         <v>19.0</v>
       </c>
-      <c r="H13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="H13" s="5">
         <v>101.0</v>
       </c>
-      <c r="J13" s="3" t="b">
+      <c r="I13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K13" s="3">
+      <c r="J13" s="3">
         <v>10.0</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>13</v>
+      <c r="K13" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -844,7 +801,7 @@
         <v>778813.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" si="1"/>
@@ -860,20 +817,17 @@
       <c r="G14" s="5">
         <v>49.0</v>
       </c>
-      <c r="H14" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="H14" s="5">
         <v>101.0</v>
       </c>
-      <c r="J14" s="3" t="b">
+      <c r="I14" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K14" s="3">
+      <c r="J14" s="3">
         <v>20.0</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>13</v>
+      <c r="K14" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
datamismatch, dont know how to fix this, ignore for now
</commit_message>
<xml_diff>
--- a/Web/db_data/testarticles.xlsx
+++ b/Web/db_data/testarticles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">lio_id</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z41</t>
   </si>
   <si>
     <t xml:space="preserve">output_per_input</t>
@@ -92,10 +89,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -171,7 +167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,10 +189,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,16 +216,16 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.7"/>
@@ -264,11 +256,8 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,11 +265,11 @@
         <v>778801</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="str">
         <f aca="false">B2</f>
-        <v>Akupunkturnålar </v>
+        <v>Akupunkturnålar</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>101</v>
@@ -301,11 +290,11 @@
         <v>778802</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="str">
         <f aca="false">B3</f>
-        <v>Urindroppsamlare </v>
+        <v>Urindroppsamlare</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>102</v>
@@ -316,10 +305,6 @@
       </c>
       <c r="G3" s="5" t="n">
         <v>39</v>
-      </c>
-      <c r="H3" s="6" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>10</v>
@@ -330,7 +315,7 @@
         <v>778803</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="str">
         <f aca="false">B4</f>
@@ -355,7 +340,7 @@
         <v>778804</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="str">
         <f aca="false">B5</f>
@@ -380,13 +365,13 @@
         <v>778805</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="str">
         <f aca="false">B6</f>
         <v>Vaccumrör Blå</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3" t="n">
         <f aca="false">A6+111100</f>
         <v>889905</v>
@@ -403,7 +388,7 @@
         <v>778806</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="str">
         <f aca="false">B7</f>
@@ -428,11 +413,11 @@
         <v>778807</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="str">
         <f aca="false">B8</f>
-        <v>Portnål </v>
+        <v>Portnål</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>105</v>
@@ -443,10 +428,6 @@
       </c>
       <c r="G8" s="5" t="n">
         <v>19</v>
-      </c>
-      <c r="H8" s="6" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I8" s="3" t="n">
         <v>10</v>
@@ -457,11 +438,11 @@
         <v>778808</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="str">
         <f aca="false">B9</f>
-        <v>Syrgasmask </v>
+        <v>Syrgasmask</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>106</v>
@@ -472,10 +453,6 @@
       </c>
       <c r="G9" s="5" t="n">
         <v>39</v>
-      </c>
-      <c r="H9" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>20</v>
@@ -486,11 +463,11 @@
         <v>778809</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="str">
         <f aca="false">B10</f>
-        <v>Trachealkanyl </v>
+        <v>Trachealkanyl</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>107</v>
@@ -501,10 +478,6 @@
       </c>
       <c r="G10" s="3" t="n">
         <v>29</v>
-      </c>
-      <c r="H10" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I10" s="3" t="n">
         <v>20</v>
@@ -515,7 +488,7 @@
         <v>778810</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="str">
         <f aca="false">B11</f>
@@ -540,11 +513,11 @@
         <v>778811</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="str">
         <f aca="false">B12</f>
-        <v>Lancett </v>
+        <v>Lancett</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>109</v>
@@ -565,11 +538,11 @@
         <v>778812</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="str">
         <f aca="false">B13</f>
-        <v>Provtagningskanyl </v>
+        <v>Provtagningskanyl</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>103</v>
@@ -580,10 +553,6 @@
       </c>
       <c r="G13" s="5" t="n">
         <v>19</v>
-      </c>
-      <c r="H13" s="6" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I13" s="3" t="n">
         <v>10</v>
@@ -594,11 +563,11 @@
         <v>778813</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="str">
         <f aca="false">B14</f>
-        <v>Blodgasspruta </v>
+        <v>Blodgasspruta</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>103</v>
@@ -609,10 +578,6 @@
       </c>
       <c r="G14" s="5" t="n">
         <v>49</v>
-      </c>
-      <c r="H14" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I14" s="3" t="n">
         <v>20</v>

</xml_diff>

<commit_message>
string length constrain (30)
</commit_message>
<xml_diff>
--- a/Web/db_data/testarticles.xlsx
+++ b/Web/db_data/testarticles.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Vaccumrör Blå</t>
   </si>
   <si>
-    <t xml:space="preserve">Natriumkloridlösning 9mg/ml 10ml</t>
+    <t xml:space="preserve">Natriumkloridlösning 9mg/10ml</t>
   </si>
   <si>
     <t xml:space="preserve">Portnål </t>
@@ -216,10 +216,10 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.14"/>
@@ -269,7 +269,7 @@
       </c>
       <c r="C2" s="3" t="str">
         <f aca="false">B2</f>
-        <v>Akupunkturnålar </v>
+        <v>Akupunkturnålar</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>101</v>
@@ -294,7 +294,7 @@
       </c>
       <c r="C3" s="3" t="str">
         <f aca="false">B3</f>
-        <v>Urindroppsamlare </v>
+        <v>Urindroppsamlare</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>102</v>
@@ -392,7 +392,7 @@
       </c>
       <c r="C7" s="3" t="str">
         <f aca="false">B7</f>
-        <v>Natriumkloridlösning 9mg/ml 10ml</v>
+        <v>Natriumkloridlösning 9mg/10ml</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>104</v>
@@ -417,7 +417,7 @@
       </c>
       <c r="C8" s="3" t="str">
         <f aca="false">B8</f>
-        <v>Portnål </v>
+        <v>Portnål</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>105</v>
@@ -442,7 +442,7 @@
       </c>
       <c r="C9" s="3" t="str">
         <f aca="false">B9</f>
-        <v>Syrgasmask </v>
+        <v>Syrgasmask</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>106</v>
@@ -467,7 +467,7 @@
       </c>
       <c r="C10" s="3" t="str">
         <f aca="false">B10</f>
-        <v>Trachealkanyl </v>
+        <v>Trachealkanyl</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>107</v>
@@ -517,7 +517,7 @@
       </c>
       <c r="C12" s="3" t="str">
         <f aca="false">B12</f>
-        <v>Lancett </v>
+        <v>Lancett</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>109</v>
@@ -542,7 +542,7 @@
       </c>
       <c r="C13" s="3" t="str">
         <f aca="false">B13</f>
-        <v>Provtagningskanyl </v>
+        <v>Provtagningskanyl</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>103</v>
@@ -567,7 +567,7 @@
       </c>
       <c r="C14" s="3" t="str">
         <f aca="false">B14</f>
-        <v>Blodgasspruta </v>
+        <v>Blodgasspruta</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>103</v>

</xml_diff>

<commit_message>
not null constraint, trying to fix Z41
</commit_message>
<xml_diff>
--- a/Web/db_data/testarticles.xlsx
+++ b/Web/db_data/testarticles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t xml:space="preserve">lio_id</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">supplier_article_nr</t>
   </si>
   <si>
+    <t xml:space="preserve">Z41</t>
+  </si>
+  <si>
     <t xml:space="preserve">image</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Urindroppsamlare </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">Vaccumrör Rosa</t>
@@ -89,9 +95,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -167,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -180,6 +187,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,6 +201,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -213,10 +228,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,336 +265,364 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>778801</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="str">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <f aca="false">B2</f>
         <v>Akupunkturnålar</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>101</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <f aca="false">A2+111100</f>
         <v>889901</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="F2" s="4"/>
+      <c r="G2" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>778802</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="str">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="str">
         <f aca="false">B3</f>
         <v>Urindroppsamlare</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>102</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <f aca="false">A3+111100</f>
         <v>889902</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>778803</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="str">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="str">
         <f aca="false">B4</f>
         <v>Vaccumrör Rosa</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <f aca="false">A4+111100</f>
         <v>889903</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="F4" s="4"/>
+      <c r="G4" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>778804</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="str">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="str">
         <f aca="false">B5</f>
         <v>Vaccumrör Grön</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <f aca="false">A5+111100</f>
         <v>889904</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="F5" s="4"/>
+      <c r="G5" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="4" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="4" t="n">
         <v>778805</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="str">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="str">
         <f aca="false">B6</f>
         <v>Vaccumrör Blå</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3" t="n">
+      <c r="D6" s="8"/>
+      <c r="E6" s="4" t="n">
         <f aca="false">A6+111100</f>
         <v>889905</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="F6" s="4"/>
+      <c r="G6" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="4" t="n">
         <v>778806</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="str">
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="str">
         <f aca="false">B7</f>
         <v>Natriumkloridlösning 9mg/10ml</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
         <v>104</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <f aca="false">A7+111100</f>
         <v>889906</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="F7" s="4"/>
+      <c r="G7" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="4" t="n">
         <v>778807</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="str">
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="str">
         <f aca="false">B8</f>
         <v>Portnål</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>105</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <f aca="false">A8+111100</f>
         <v>889907</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="4" t="n">
         <v>778808</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="str">
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="str">
         <f aca="false">B9</f>
         <v>Syrgasmask</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="5" t="n">
         <v>106</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <f aca="false">A9+111100</f>
         <v>889908</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="4" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="4" t="n">
         <v>778809</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="str">
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="str">
         <f aca="false">B10</f>
         <v>Trachealkanyl</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="5" t="n">
         <v>107</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <f aca="false">A10+111100</f>
         <v>889909</v>
       </c>
-      <c r="G10" s="3" t="n">
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="4" t="n">
         <v>778810</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="str">
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="str">
         <f aca="false">B11</f>
         <v>Elastisk viskosstrumpa</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>108</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <f aca="false">A11+111100</f>
         <v>889910</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="F11" s="4"/>
+      <c r="G11" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="H11" s="3" t="n">
+      <c r="H11" s="4" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="4" t="n">
         <v>778811</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="str">
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="str">
         <f aca="false">B12</f>
         <v>Lancett</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>109</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="4" t="n">
         <f aca="false">A12+111100</f>
         <v>889911</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="F12" s="4"/>
+      <c r="G12" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="4" t="n">
         <v>250</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="4" t="n">
         <v>778812</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="3" t="str">
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="str">
         <f aca="false">B13</f>
         <v>Provtagningskanyl</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="4" t="n">
         <f aca="false">A13+111100</f>
         <v>889912</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="F13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="4" t="n">
         <v>778813</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3" t="str">
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="str">
         <f aca="false">B14</f>
         <v>Blodgasspruta</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="4" t="n">
         <f aca="false">A14+111100</f>
         <v>889913</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="6" t="n">
         <v>49</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
panda should not convert true to 1.0
</commit_message>
<xml_diff>
--- a/Web/db_data/testarticles.xlsx
+++ b/Web/db_data/testarticles.xlsx
@@ -95,10 +95,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -174,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,11 +200,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,7 +236,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -296,8 +301,10 @@
         <f aca="false">A2+111100</f>
         <v>889901</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="6" t="n">
+      <c r="F2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="n">
         <v>29</v>
       </c>
       <c r="H2" s="4" t="n">
@@ -322,10 +329,10 @@
         <f aca="false">A3+111100</f>
         <v>889902</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="7" t="n">
         <v>39</v>
       </c>
       <c r="H3" s="4" t="n">
@@ -350,8 +357,10 @@
         <f aca="false">A4+111100</f>
         <v>889903</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="6" t="n">
+      <c r="F4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="n">
         <v>19</v>
       </c>
       <c r="H4" s="4" t="n">
@@ -376,8 +385,10 @@
         <f aca="false">A5+111100</f>
         <v>889904</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="6" t="n">
+      <c r="F5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="n">
         <v>19</v>
       </c>
       <c r="H5" s="4" t="n">
@@ -395,13 +406,15 @@
         <f aca="false">B6</f>
         <v>Vaccumrör Blå</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="4" t="n">
         <f aca="false">A6+111100</f>
         <v>889905</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6" t="n">
+      <c r="F6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="n">
         <v>19</v>
       </c>
       <c r="H6" s="4" t="n">
@@ -426,8 +439,10 @@
         <f aca="false">A7+111100</f>
         <v>889906</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6" t="n">
+      <c r="F7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="n">
         <v>29</v>
       </c>
       <c r="H7" s="4" t="n">
@@ -452,10 +467,10 @@
         <f aca="false">A8+111100</f>
         <v>889907</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>19</v>
       </c>
       <c r="H8" s="4" t="n">
@@ -480,10 +495,10 @@
         <f aca="false">A9+111100</f>
         <v>889908</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="7" t="n">
         <v>39</v>
       </c>
       <c r="H9" s="4" t="n">
@@ -508,7 +523,7 @@
         <f aca="false">A10+111100</f>
         <v>889909</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="4" t="n">
@@ -536,8 +551,10 @@
         <f aca="false">A11+111100</f>
         <v>889910</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="6" t="n">
+      <c r="F11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="n">
         <v>39</v>
       </c>
       <c r="H11" s="4" t="n">
@@ -562,8 +579,10 @@
         <f aca="false">A12+111100</f>
         <v>889911</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="6" t="n">
+      <c r="F12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="n">
         <v>39</v>
       </c>
       <c r="H12" s="4" t="n">
@@ -588,10 +607,10 @@
         <f aca="false">A13+111100</f>
         <v>889912</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="6" t="n">
+      <c r="G13" s="7" t="n">
         <v>19</v>
       </c>
       <c r="H13" s="4" t="n">
@@ -616,10 +635,10 @@
         <f aca="false">A14+111100</f>
         <v>889913</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="6" t="n">
+      <c r="G14" s="7" t="n">
         <v>49</v>
       </c>
       <c r="H14" s="4" t="n">

</xml_diff>